<commit_message>
formatted everything into gram
</commit_message>
<xml_diff>
--- a/data/food.xlsx
+++ b/data/food.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$23</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,10 +73,10 @@
     <t xml:space="preserve">MJ per Kg of Product</t>
   </si>
   <si>
-    <t xml:space="preserve">L per Kg of product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calories in 100g</t>
+    <t xml:space="preserve">L per g of product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calories in 1g</t>
   </si>
   <si>
     <t xml:space="preserve">in g</t>
@@ -320,7 +321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,8 +350,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -374,23 +383,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,7 +489,7 @@
         <v>26.309886088216</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>5000</v>
+        <v>5000000</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>19</v>
@@ -488,8 +497,8 @@
       <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="n">
-        <v>576</v>
+      <c r="G3" s="7" t="n">
+        <v>5.76</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>50</v>
@@ -517,7 +526,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3" t="n">
-        <v>200</v>
+        <v>200000</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>
@@ -525,8 +534,8 @@
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4" t="n">
-        <v>52</v>
+      <c r="G4" s="7" t="n">
+        <v>0.52</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>0.2</v>
@@ -554,7 +563,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="n">
-        <v>900</v>
+        <v>900000</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
@@ -562,8 +571,8 @@
       <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="4" t="n">
-        <v>89</v>
+      <c r="G5" s="7" t="n">
+        <v>0.89</v>
       </c>
       <c r="H5" s="4" t="n">
         <v>0.3</v>
@@ -585,7 +594,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="6" t="n">
@@ -595,7 +604,7 @@
         <v>164.224859803377</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>15415</v>
+        <v>15415000</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
@@ -603,8 +612,8 @@
       <c r="F6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="4" t="n">
-        <v>198</v>
+      <c r="G6" s="7" t="n">
+        <v>1.98</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>13</v>
@@ -632,7 +641,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="n">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>19</v>
@@ -640,8 +649,8 @@
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="3" t="n">
-        <v>267</v>
+      <c r="G7" s="9" t="n">
+        <v>2.67</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>3.2</v>
@@ -663,7 +672,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="3" t="n">
@@ -671,7 +680,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="n">
-        <v>5553</v>
+        <v>5553000</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>30</v>
@@ -679,8 +688,8 @@
       <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="4" t="n">
-        <v>717</v>
+      <c r="G8" s="7" t="n">
+        <v>7.17</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>81</v>
@@ -708,7 +717,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3" t="n">
-        <v>455</v>
+        <v>455000</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
@@ -716,8 +725,8 @@
       <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="3" t="n">
-        <v>25</v>
+      <c r="G9" s="9" t="n">
+        <v>0.25</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>0.1</v>
@@ -745,7 +754,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="n">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
@@ -753,8 +762,8 @@
       <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="3" t="n">
-        <v>41</v>
+      <c r="G10" s="9" t="n">
+        <v>0.41</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>0.2</v>
@@ -776,7 +785,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6" t="n">
@@ -786,7 +795,7 @@
         <v>35.4955782619731</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>3178</v>
+        <v>3178000</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>30</v>
@@ -794,8 +803,8 @@
       <c r="F11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="3" t="n">
-        <v>393</v>
+      <c r="G11" s="9" t="n">
+        <v>3.93</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>31</v>
@@ -817,7 +826,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="6" t="n">
@@ -827,7 +836,7 @@
         <v>64.135317267657</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>4325</v>
+        <v>4325000</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
@@ -835,8 +844,8 @@
       <c r="F12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="3" t="n">
-        <v>158</v>
+      <c r="G12" s="9" t="n">
+        <v>1.58</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>18</v>
@@ -858,7 +867,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="3" t="n">
@@ -866,7 +875,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4" t="n">
-        <v>10157.3621651</v>
+        <v>10157362.1651</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
@@ -874,8 +883,8 @@
       <c r="F13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="3" t="n">
-        <v>139</v>
+      <c r="G13" s="9" t="n">
+        <v>1.39</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>2.8</v>
@@ -897,7 +906,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="6" t="n">
@@ -907,7 +916,7 @@
         <v>1.87664233710806</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>892.958583926</v>
+        <v>892958.583926</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
@@ -915,8 +924,8 @@
       <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="3" t="n">
-        <v>365</v>
+      <c r="G14" s="9" t="n">
+        <v>3.65</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>4.7</v>
@@ -944,7 +953,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3" t="n">
-        <v>555</v>
+        <v>555000</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
@@ -952,8 +961,8 @@
       <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="3" t="n">
-        <v>12</v>
+      <c r="G15" s="9" t="n">
+        <v>0.12</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>0.2</v>
@@ -975,7 +984,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="6" t="n">
@@ -985,7 +994,7 @@
         <v>17.2256703244356</v>
       </c>
       <c r="D16" s="6" t="n">
-        <v>1849</v>
+        <v>1849000</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -993,8 +1002,8 @@
       <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="3" t="n">
-        <v>352</v>
+      <c r="G16" s="9" t="n">
+        <v>3.52</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>2.9</v>
@@ -1016,7 +1025,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="6" t="n">
@@ -1026,14 +1035,14 @@
         <v>36.0993272341019</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>3000</v>
+        <v>3000000</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="3" t="n">
-        <v>196</v>
+      <c r="G17" s="9" t="n">
+        <v>1.96</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>15</v>
@@ -1061,7 +1070,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="n">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>19</v>
@@ -1069,8 +1078,8 @@
       <c r="F18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="3" t="n">
-        <v>242</v>
+      <c r="G18" s="9" t="n">
+        <v>2.42</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>0.2</v>
@@ -1092,7 +1101,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="3" t="n">
@@ -1100,7 +1109,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4" t="n">
-        <v>10412</v>
+        <v>10412000</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>26</v>
@@ -1108,8 +1117,8 @@
       <c r="F19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="3" t="n">
-        <v>282</v>
+      <c r="G19" s="9" t="n">
+        <v>2.82</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>23</v>
@@ -1131,7 +1140,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="6" t="n">
@@ -1141,7 +1150,7 @@
         <v>5.67374478926682</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>19</v>
@@ -1149,8 +1158,8 @@
       <c r="F20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="3" t="n">
-        <v>352</v>
+      <c r="G20" s="9" t="n">
+        <v>3.52</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>1.1</v>
@@ -1178,7 +1187,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="3" t="n">
-        <v>500</v>
+        <v>500000</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>19</v>
@@ -1186,8 +1195,8 @@
       <c r="F21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="3" t="n">
-        <v>15</v>
+      <c r="G21" s="9" t="n">
+        <v>0.15</v>
       </c>
       <c r="H21" s="3" t="n">
         <v>0.2</v>
@@ -1209,7 +1218,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="6" t="n">
@@ -1219,7 +1228,7 @@
         <v>1.38938571246988</v>
       </c>
       <c r="D22" s="6" t="n">
-        <v>3500</v>
+        <v>3500000</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>30</v>
@@ -1227,8 +1236,8 @@
       <c r="F22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="3" t="n">
-        <v>61</v>
+      <c r="G22" s="9" t="n">
+        <v>0.61</v>
       </c>
       <c r="H22" s="3" t="n">
         <v>3.5</v>
@@ -1256,7 +1265,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="3" t="n">
-        <v>3025</v>
+        <v>3025000</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>19</v>
@@ -1264,8 +1273,8 @@
       <c r="F23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="3" t="n">
-        <v>145</v>
+      <c r="G23" s="9" t="n">
+        <v>1.45</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>15</v>
@@ -1293,7 +1302,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="n">
-        <v>1500</v>
+        <v>1500000</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>19</v>
@@ -1301,8 +1310,8 @@
       <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="3" t="n">
-        <v>884</v>
+      <c r="G24" s="9" t="n">
+        <v>8.84</v>
       </c>
       <c r="H24" s="3" t="n">
         <v>100</v>
@@ -1330,7 +1339,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="n">
-        <v>400</v>
+        <v>400000</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>19</v>
@@ -1338,8 +1347,8 @@
       <c r="F25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="3" t="n">
-        <v>40</v>
+      <c r="G25" s="9" t="n">
+        <v>0.4</v>
       </c>
       <c r="H25" s="3" t="n">
         <v>0.1</v>
@@ -1367,7 +1376,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="3" t="n">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>19</v>
@@ -1375,8 +1384,8 @@
       <c r="F26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="3" t="n">
-        <v>46</v>
+      <c r="G26" s="9" t="n">
+        <v>0.46</v>
       </c>
       <c r="H26" s="3" t="n">
         <v>0.2</v>
@@ -1404,7 +1413,7 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="n">
-        <v>9001</v>
+        <v>9001000</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>19</v>
@@ -1412,8 +1421,8 @@
       <c r="F27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="3" t="n">
-        <v>884</v>
+      <c r="G27" s="9" t="n">
+        <v>8.84</v>
       </c>
       <c r="H27" s="3" t="n">
         <v>100</v>
@@ -1435,7 +1444,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="3" t="n">
@@ -1443,7 +1452,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="n">
-        <v>5945.93581192</v>
+        <v>5945935.81192</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>19</v>
@@ -1451,8 +1460,8 @@
       <c r="F28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="3" t="n">
-        <v>81</v>
+      <c r="G28" s="9" t="n">
+        <v>0.81</v>
       </c>
       <c r="H28" s="3" t="n">
         <v>0.4</v>
@@ -1474,7 +1483,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="6" t="n">
@@ -1484,7 +1493,7 @@
         <v>91.4018076048471</v>
       </c>
       <c r="D29" s="6" t="n">
-        <v>5988</v>
+        <v>5988000</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>26</v>
@@ -1492,8 +1501,8 @@
       <c r="F29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="3" t="n">
-        <v>263</v>
+      <c r="G29" s="9" t="n">
+        <v>2.63</v>
       </c>
       <c r="H29" s="3" t="n">
         <v>21</v>
@@ -1521,7 +1530,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="3" t="n">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>19</v>
@@ -1529,8 +1538,8 @@
       <c r="F30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="3" t="n">
-        <v>77</v>
+      <c r="G30" s="9" t="n">
+        <v>0.77</v>
       </c>
       <c r="H30" s="3" t="n">
         <v>0.1</v>
@@ -1552,7 +1561,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="3" t="n">
@@ -1560,7 +1569,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="n">
-        <v>5000</v>
+        <v>5000000</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>26</v>
@@ -1568,8 +1577,8 @@
       <c r="F31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="3" t="n">
-        <v>114</v>
+      <c r="G31" s="9" t="n">
+        <v>1.14</v>
       </c>
       <c r="H31" s="3" t="n">
         <v>2.3</v>
@@ -1591,7 +1600,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="6" t="n">
@@ -1601,7 +1610,7 @@
         <v>5.67374478926682</v>
       </c>
       <c r="D32" s="6" t="n">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>19</v>
@@ -1609,8 +1618,8 @@
       <c r="F32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="3" t="n">
-        <v>124</v>
+      <c r="G32" s="9" t="n">
+        <v>1.24</v>
       </c>
       <c r="H32" s="3" t="n">
         <v>1.1</v>
@@ -1632,7 +1641,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="6" t="n">
@@ -1642,7 +1651,7 @@
         <v>5.42924104539067</v>
       </c>
       <c r="D33" s="6" t="n">
-        <v>2497</v>
+        <v>2497000</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>19</v>
@@ -1650,8 +1659,8 @@
       <c r="F33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="3" t="n">
-        <v>367</v>
+      <c r="G33" s="9" t="n">
+        <v>3.67</v>
       </c>
       <c r="H33" s="3" t="n">
         <v>3.2</v>
@@ -1673,7 +1682,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="6" t="n">
@@ -1683,7 +1692,7 @@
         <v>0.257129871380158</v>
       </c>
       <c r="D34" s="6" t="n">
-        <v>2500</v>
+        <v>2500000</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>19</v>
@@ -1691,8 +1700,8 @@
       <c r="F34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G34" s="3" t="n">
-        <v>47</v>
+      <c r="G34" s="9" t="n">
+        <v>0.47</v>
       </c>
       <c r="H34" s="3" t="n">
         <v>1</v>
@@ -1714,7 +1723,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B35" s="6" t="n">
@@ -1724,7 +1733,7 @@
         <v>14.366381167705</v>
       </c>
       <c r="D35" s="6" t="n">
-        <v>2036.27938764</v>
+        <v>2036279.38764</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>19</v>
@@ -1732,8 +1741,8 @@
       <c r="F35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="3" t="n">
-        <v>270</v>
+      <c r="G35" s="9" t="n">
+        <v>2.7</v>
       </c>
       <c r="H35" s="3" t="n">
         <v>20</v>
@@ -1761,7 +1770,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="3" t="n">
-        <v>600</v>
+        <v>600000</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>19</v>
@@ -1769,8 +1778,8 @@
       <c r="F36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="3" t="n">
-        <v>32</v>
+      <c r="G36" s="9" t="n">
+        <v>0.32</v>
       </c>
       <c r="H36" s="3" t="n">
         <v>0.3</v>
@@ -1792,7 +1801,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B37" s="3" t="n">
@@ -1800,7 +1809,7 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="n">
-        <v>6000</v>
+        <v>6000000</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>26</v>
@@ -1808,8 +1817,8 @@
       <c r="F37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="3" t="n">
-        <v>112</v>
+      <c r="G37" s="9" t="n">
+        <v>1.12</v>
       </c>
       <c r="H37" s="3" t="n">
         <v>1.9</v>
@@ -1830,8 +1839,13 @@
         <v>0.067</v>
       </c>
     </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M37"/>
+  <autoFilter ref="A1:G31"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fixed food.xlsx to have values for 1g
</commit_message>
<xml_diff>
--- a/data/food.xlsx
+++ b/data/food.xlsx
@@ -11,10 +11,11 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$D$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$M$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$G$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$D$23</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -386,20 +387,20 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="O26" activeCellId="0" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,19 +502,19 @@
         <v>5.76</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>0.001</v>
+        <v>1E-005</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>4.4</v>
+        <v>0.044</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>0</v>
@@ -538,19 +539,19 @@
         <v>0.52</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>0.001</v>
+        <v>1E-005</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0.3</v>
+        <v>0.003</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>0</v>
@@ -575,19 +576,19 @@
         <v>0.89</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>0.3</v>
+        <v>0.003</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>0.001</v>
+        <v>1E-005</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>1.1</v>
+        <v>0.011</v>
       </c>
       <c r="M5" s="3" t="n">
         <v>0</v>
@@ -616,10 +617,10 @@
         <v>1.98</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>0.068</v>
+        <v>0.00068</v>
       </c>
       <c r="J6" s="3" t="n">
         <v>0</v>
@@ -628,10 +629,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>0.062</v>
+        <v>0.00062</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,19 +654,19 @@
         <v>2.67</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>3.2</v>
+        <v>0.032</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>0.508</v>
+        <v>0.00508</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>5.9</v>
+        <v>0.059</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>49</v>
+        <v>0.49</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="M7" s="3" t="n">
         <v>0</v>
@@ -692,22 +693,22 @@
         <v>7.17</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>81</v>
+        <v>0.81</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>0.643</v>
+        <v>0.00643</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>0.9</v>
+        <v>0.009</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>0.215</v>
+        <v>0.00215</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,19 +730,19 @@
         <v>0.25</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>0.018</v>
+        <v>0.00018</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>3.2</v>
+        <v>0.032</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>5.8</v>
+        <v>0.058</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>1.3</v>
+        <v>0.013</v>
       </c>
       <c r="M9" s="3" t="n">
         <v>0</v>
@@ -766,19 +767,19 @@
         <v>0.41</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>0.69</v>
+        <v>0.0069</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>4.7</v>
+        <v>0.047</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>9.6</v>
+        <v>0.096</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0.9</v>
+        <v>0.009</v>
       </c>
       <c r="M10" s="3" t="n">
         <v>0</v>
@@ -807,22 +808,22 @@
         <v>3.93</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>31</v>
+        <v>0.31</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>0.187</v>
+        <v>0.00187</v>
       </c>
       <c r="J11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>1.4</v>
+        <v>0.014</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>27</v>
+        <v>0.27</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>0.093</v>
+        <v>0.00093</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,22 +849,22 @@
         <v>1.58</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>0.722</v>
+        <v>0.00722</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>0.5</v>
+        <v>0.005</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>4.1</v>
+        <v>0.041</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>0.056</v>
+        <v>0.00056</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,19 +888,19 @@
         <v>1.39</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>2.8</v>
+        <v>0.028</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>0.246</v>
+        <v>0.00246</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="K13" s="3" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>7.1</v>
+        <v>0.071</v>
       </c>
       <c r="M13" s="3" t="n">
         <v>0</v>
@@ -928,19 +929,19 @@
         <v>3.65</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>4.7</v>
+        <v>0.047</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>0.035</v>
+        <v>0.00035</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>0.6</v>
+        <v>0.006</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>74</v>
+        <v>0.74</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>9.4</v>
+        <v>0.094</v>
       </c>
       <c r="M14" s="3" t="n">
         <v>0</v>
@@ -965,19 +966,19 @@
         <v>0.12</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>0.002</v>
+        <v>2E-005</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>1.4</v>
+        <v>0.014</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>2.2</v>
+        <v>0.022</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>0.6</v>
+        <v>0.006</v>
       </c>
       <c r="M15" s="3" t="n">
         <v>0</v>
@@ -1006,19 +1007,19 @@
         <v>3.52</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>2.9</v>
+        <v>0.029</v>
       </c>
       <c r="I16" s="3" t="n">
-        <v>0.006</v>
+        <v>6E-005</v>
       </c>
       <c r="J16" s="3" t="n">
-        <v>2.7</v>
+        <v>0.027</v>
       </c>
       <c r="K16" s="3" t="n">
-        <v>73</v>
+        <v>0.73</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="M16" s="3" t="n">
         <v>0</v>
@@ -1045,22 +1046,22 @@
         <v>1.96</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>0.207</v>
+        <v>0.00207</v>
       </c>
       <c r="J17" s="3" t="n">
-        <v>0.4</v>
+        <v>0.004</v>
       </c>
       <c r="K17" s="3" t="n">
-        <v>0.8</v>
+        <v>0.008</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>0.401</v>
+        <v>0.00401</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,19 +1083,19 @@
         <v>2.42</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I18" s="3" t="n">
-        <v>0.04</v>
+        <v>0.0004</v>
       </c>
       <c r="J18" s="3" t="n">
-        <v>43</v>
+        <v>0.43</v>
       </c>
       <c r="K18" s="3" t="n">
-        <v>64</v>
+        <v>0.64</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>0.7</v>
+        <v>0.007</v>
       </c>
       <c r="M18" s="3" t="n">
         <v>0</v>
@@ -1121,10 +1122,10 @@
         <v>2.82</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>0.059</v>
+        <v>0.00059</v>
       </c>
       <c r="J19" s="3" t="n">
         <v>0</v>
@@ -1133,10 +1134,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="M19" s="3" t="n">
-        <v>0.073</v>
+        <v>0.00073</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,19 +1163,19 @@
         <v>3.52</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>1.1</v>
+        <v>0.011</v>
       </c>
       <c r="I20" s="3" t="n">
-        <v>0.006</v>
+        <v>6E-005</v>
       </c>
       <c r="J20" s="3" t="n">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="K20" s="3" t="n">
-        <v>63</v>
+        <v>0.63</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="M20" s="3" t="n">
         <v>0</v>
@@ -1199,19 +1200,19 @@
         <v>0.15</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I21" s="3" t="n">
-        <v>0.028</v>
+        <v>0.00028</v>
       </c>
       <c r="J21" s="3" t="n">
-        <v>0.8</v>
+        <v>0.008</v>
       </c>
       <c r="K21" s="3" t="n">
-        <v>2.9</v>
+        <v>0.029</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>1.4</v>
+        <v>0.014</v>
       </c>
       <c r="M21" s="3" t="n">
         <v>0</v>
@@ -1240,22 +1241,22 @@
         <v>0.61</v>
       </c>
       <c r="H22" s="3" t="n">
-        <v>3.5</v>
+        <v>0.035</v>
       </c>
       <c r="I22" s="3" t="n">
-        <v>0.003</v>
+        <v>3E-005</v>
       </c>
       <c r="J22" s="3" t="n">
-        <v>4.5</v>
+        <v>0.045</v>
       </c>
       <c r="K22" s="3" t="n">
-        <v>4.5</v>
+        <v>0.045</v>
       </c>
       <c r="L22" s="3" t="n">
-        <v>3.1</v>
+        <v>0.031</v>
       </c>
       <c r="M22" s="3" t="n">
-        <v>0.014</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,19 +1278,19 @@
         <v>1.45</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>1.556</v>
+        <v>0.01556</v>
       </c>
       <c r="J23" s="3" t="n">
-        <v>0.5</v>
+        <v>0.005</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>3.8</v>
+        <v>0.038</v>
       </c>
       <c r="L23" s="3" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="M23" s="3" t="n">
         <v>0</v>
@@ -1314,10 +1315,10 @@
         <v>8.84</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I24" s="3" t="n">
-        <v>0.002</v>
+        <v>2E-005</v>
       </c>
       <c r="J24" s="3" t="n">
         <v>0</v>
@@ -1351,19 +1352,19 @@
         <v>0.4</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>0.004</v>
+        <v>4E-005</v>
       </c>
       <c r="J25" s="3" t="n">
-        <v>4.2</v>
+        <v>0.042</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>9.3</v>
+        <v>0.093</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>1.1</v>
+        <v>0.011</v>
       </c>
       <c r="M25" s="3" t="n">
         <v>0</v>
@@ -1388,19 +1389,19 @@
         <v>0.46</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>0.2</v>
+        <v>0.002</v>
       </c>
       <c r="I26" s="3" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="3" t="n">
-        <v>9.1</v>
+        <v>0.091</v>
       </c>
       <c r="K26" s="3" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>0.7</v>
+        <v>0.007</v>
       </c>
       <c r="M26" s="3" t="n">
         <v>0</v>
@@ -1425,7 +1426,7 @@
         <v>8.84</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I27" s="3" t="n">
         <v>0</v>
@@ -1464,19 +1465,19 @@
         <v>0.81</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>0.4</v>
+        <v>0.004</v>
       </c>
       <c r="I28" s="3" t="n">
-        <v>0.005</v>
+        <v>5E-005</v>
       </c>
       <c r="J28" s="3" t="n">
-        <v>5.7</v>
+        <v>0.057</v>
       </c>
       <c r="K28" s="3" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="L28" s="3" t="n">
-        <v>5.4</v>
+        <v>0.054</v>
       </c>
       <c r="M28" s="3" t="n">
         <v>0</v>
@@ -1505,10 +1506,10 @@
         <v>2.63</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>0.056</v>
+        <v>0.00056</v>
       </c>
       <c r="J29" s="3" t="n">
         <v>0</v>
@@ -1517,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="L29" s="3" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="M29" s="3" t="n">
-        <v>0.072</v>
+        <v>0.00072</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,19 +1543,19 @@
         <v>0.77</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="I30" s="3" t="n">
-        <v>0.006</v>
+        <v>6E-005</v>
       </c>
       <c r="J30" s="3" t="n">
-        <v>0.8</v>
+        <v>0.008</v>
       </c>
       <c r="K30" s="3" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>2.1</v>
+        <v>0.021</v>
       </c>
       <c r="M30" s="3" t="n">
         <v>0</v>
@@ -1581,10 +1582,10 @@
         <v>1.14</v>
       </c>
       <c r="H31" s="3" t="n">
-        <v>2.3</v>
+        <v>0.023</v>
       </c>
       <c r="I31" s="3" t="n">
-        <v>0.05</v>
+        <v>0.0005</v>
       </c>
       <c r="J31" s="3" t="n">
         <v>0</v>
@@ -1593,10 +1594,10 @@
         <v>0</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="M31" s="3" t="n">
-        <v>0.081</v>
+        <v>0.00081</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,19 +1623,19 @@
         <v>1.24</v>
       </c>
       <c r="H32" s="3" t="n">
-        <v>1.1</v>
+        <v>0.011</v>
       </c>
       <c r="I32" s="3" t="n">
-        <v>0.231</v>
+        <v>0.00231</v>
       </c>
       <c r="J32" s="3" t="n">
-        <v>3.8</v>
+        <v>0.038</v>
       </c>
       <c r="K32" s="3" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="L32" s="3" t="n">
-        <v>8</v>
+        <v>0.08</v>
       </c>
       <c r="M32" s="3" t="n">
         <v>0</v>
@@ -1663,19 +1664,19 @@
         <v>3.67</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>3.2</v>
+        <v>0.032</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>0.005</v>
+        <v>5E-005</v>
       </c>
       <c r="J33" s="3" t="n">
-        <v>0.7</v>
+        <v>0.007</v>
       </c>
       <c r="K33" s="3" t="n">
-        <v>76</v>
+        <v>0.76</v>
       </c>
       <c r="L33" s="3" t="n">
-        <v>7.5</v>
+        <v>0.075</v>
       </c>
       <c r="M33" s="3" t="n">
         <v>0</v>
@@ -1704,19 +1705,19 @@
         <v>0.47</v>
       </c>
       <c r="H34" s="3" t="n">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I34" s="3" t="n">
-        <v>0.039</v>
+        <v>0.00039</v>
       </c>
       <c r="J34" s="3" t="n">
-        <v>5.3</v>
+        <v>0.053</v>
       </c>
       <c r="K34" s="3" t="n">
-        <v>9.2</v>
+        <v>0.092</v>
       </c>
       <c r="L34" s="3" t="n">
-        <v>0.3</v>
+        <v>0.003</v>
       </c>
       <c r="M34" s="3" t="n">
         <v>0</v>
@@ -1745,19 +1746,19 @@
         <v>2.7</v>
       </c>
       <c r="H35" s="3" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="I35" s="3" t="n">
-        <v>0.016</v>
+        <v>0.00016</v>
       </c>
       <c r="J35" s="3" t="n">
-        <v>2.7</v>
+        <v>0.027</v>
       </c>
       <c r="K35" s="3" t="n">
-        <v>8.9</v>
+        <v>0.089</v>
       </c>
       <c r="L35" s="3" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="M35" s="3" t="n">
         <v>0</v>
@@ -1782,19 +1783,19 @@
         <v>0.32</v>
       </c>
       <c r="H36" s="3" t="n">
-        <v>0.3</v>
+        <v>0.003</v>
       </c>
       <c r="I36" s="3" t="n">
-        <v>0.186</v>
+        <v>0.00186</v>
       </c>
       <c r="J36" s="3" t="n">
-        <v>4.4</v>
+        <v>0.044</v>
       </c>
       <c r="K36" s="3" t="n">
-        <v>7.3</v>
+        <v>0.073</v>
       </c>
       <c r="L36" s="3" t="n">
-        <v>1.6</v>
+        <v>0.016</v>
       </c>
       <c r="M36" s="3" t="n">
         <v>0</v>
@@ -1821,31 +1822,31 @@
         <v>1.12</v>
       </c>
       <c r="H37" s="3" t="n">
-        <v>1.9</v>
+        <v>0.019</v>
       </c>
       <c r="I37" s="3" t="n">
-        <v>0.118</v>
+        <v>0.00118</v>
       </c>
       <c r="J37" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="K37" s="3" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="M37" s="3" t="n">
-        <v>0.067</v>
+        <v>0.00067</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H48" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G31"/>
+  <autoFilter ref="A1:M37"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>